<commit_message>
Connections now render on Connections page
</commit_message>
<xml_diff>
--- a/References/Tidsplan.xlsx
+++ b/References/Tidsplan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1516C6C-1A85-44AF-B6CB-F2D4B9549DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA062C4-CD4A-403D-9858-24413AD5D43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravspecifikation" sheetId="13" r:id="rId1"/>
@@ -1240,23 +1240,23 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2576,9 +2576,9 @@
   </sheetPr>
   <dimension ref="A1:CC43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2634,127 +2634,127 @@
       <c r="C3" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="112"/>
-      <c r="F3" s="116">
+      <c r="E3" s="116"/>
+      <c r="F3" s="114">
         <f>DATE(2022,9,19)</f>
         <v>44823</v>
       </c>
-      <c r="G3" s="116"/>
+      <c r="G3" s="114"/>
     </row>
     <row r="4" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="112"/>
+      <c r="E4" s="116"/>
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="113">
+      <c r="L4" s="111">
         <f>L5</f>
         <v>44823</v>
       </c>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="113">
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="111">
         <f>S5</f>
         <v>44830</v>
       </c>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="115"/>
-      <c r="Z4" s="113">
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="112"/>
+      <c r="Y4" s="113"/>
+      <c r="Z4" s="111">
         <f>Z5</f>
         <v>44837</v>
       </c>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="114"/>
-      <c r="AF4" s="115"/>
-      <c r="AG4" s="113">
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="113"/>
+      <c r="AG4" s="111">
         <f>AG5</f>
         <v>44844</v>
       </c>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="114"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="113">
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="112"/>
+      <c r="AM4" s="113"/>
+      <c r="AN4" s="111">
         <f>AN5</f>
         <v>44851</v>
       </c>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="114"/>
-      <c r="AT4" s="115"/>
-      <c r="AU4" s="113">
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="112"/>
+      <c r="AT4" s="113"/>
+      <c r="AU4" s="111">
         <f>AU5</f>
         <v>44858</v>
       </c>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="114"/>
-      <c r="BA4" s="115"/>
-      <c r="BB4" s="113">
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="112"/>
+      <c r="BA4" s="113"/>
+      <c r="BB4" s="111">
         <f>BB5</f>
         <v>44865</v>
       </c>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114"/>
-      <c r="BF4" s="114"/>
-      <c r="BG4" s="114"/>
-      <c r="BH4" s="115"/>
-      <c r="BI4" s="113">
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="112"/>
+      <c r="BG4" s="112"/>
+      <c r="BH4" s="113"/>
+      <c r="BI4" s="111">
         <f>BI5</f>
         <v>44872</v>
       </c>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="114"/>
-      <c r="BM4" s="114"/>
-      <c r="BN4" s="114"/>
-      <c r="BO4" s="115"/>
-      <c r="BP4" s="113">
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="112"/>
+      <c r="BN4" s="112"/>
+      <c r="BO4" s="113"/>
+      <c r="BP4" s="111">
         <f>BP5</f>
         <v>44879</v>
       </c>
-      <c r="BQ4" s="114"/>
-      <c r="BR4" s="114"/>
-      <c r="BS4" s="114"/>
-      <c r="BT4" s="114"/>
-      <c r="BU4" s="114"/>
-      <c r="BV4" s="115"/>
-      <c r="BW4" s="113">
+      <c r="BQ4" s="112"/>
+      <c r="BR4" s="112"/>
+      <c r="BS4" s="112"/>
+      <c r="BT4" s="112"/>
+      <c r="BU4" s="112"/>
+      <c r="BV4" s="113"/>
+      <c r="BW4" s="111">
         <f>BW5</f>
         <v>44886</v>
       </c>
-      <c r="BX4" s="114"/>
-      <c r="BY4" s="114"/>
-      <c r="BZ4" s="114"/>
-      <c r="CA4" s="114"/>
-      <c r="CB4" s="114"/>
-      <c r="CC4" s="115"/>
+      <c r="BX4" s="112"/>
+      <c r="BY4" s="112"/>
+      <c r="BZ4" s="112"/>
+      <c r="CA4" s="112"/>
+      <c r="CB4" s="112"/>
+      <c r="CC4" s="113"/>
     </row>
     <row r="5" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
@@ -6712,6 +6712,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="AN4:AT4"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BP4:BV4"/>
     <mergeCell ref="BW4:CC4"/>
     <mergeCell ref="BI4:BO4"/>
@@ -6720,11 +6725,6 @@
     <mergeCell ref="S4:Y4"/>
     <mergeCell ref="Z4:AF4"/>
     <mergeCell ref="AG4:AM4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="AN4:AT4"/>
-    <mergeCell ref="AU4:BA4"/>
-    <mergeCell ref="BB4:BH4"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E40">
     <cfRule type="dataBar" priority="71">

</xml_diff>

<commit_message>
If only I could get camera to work
</commit_message>
<xml_diff>
--- a/References/Tidsplan.xlsx
+++ b/References/Tidsplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA062C4-CD4A-403D-9858-24413AD5D43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB1E4BD-6474-439C-AAD7-EB7338EBAC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1240,6 +1240,12 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1251,12 +1257,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2576,9 +2576,9 @@
   </sheetPr>
   <dimension ref="A1:CC43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AV6" sqref="AV6"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BD1" sqref="BD1:BD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2634,127 +2634,127 @@
       <c r="C3" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="116"/>
-      <c r="F3" s="114">
+      <c r="E3" s="112"/>
+      <c r="F3" s="116">
         <f>DATE(2022,9,19)</f>
         <v>44823</v>
       </c>
-      <c r="G3" s="114"/>
+      <c r="G3" s="116"/>
     </row>
     <row r="4" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="116"/>
+      <c r="E4" s="112"/>
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="111">
+      <c r="L4" s="113">
         <f>L5</f>
         <v>44823</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="111">
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="113">
         <f>S5</f>
         <v>44830</v>
       </c>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="113"/>
-      <c r="Z4" s="111">
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="114"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="113">
         <f>Z5</f>
         <v>44837</v>
       </c>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="113"/>
-      <c r="AG4" s="111">
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="114"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="113">
         <f>AG5</f>
         <v>44844</v>
       </c>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="112"/>
-      <c r="AM4" s="113"/>
-      <c r="AN4" s="111">
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="114"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="113">
         <f>AN5</f>
         <v>44851</v>
       </c>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="112"/>
-      <c r="AT4" s="113"/>
-      <c r="AU4" s="111">
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="114"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="113">
         <f>AU5</f>
         <v>44858</v>
       </c>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="112"/>
-      <c r="BA4" s="113"/>
-      <c r="BB4" s="111">
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="114"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="113">
         <f>BB5</f>
         <v>44865</v>
       </c>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="112"/>
-      <c r="BH4" s="113"/>
-      <c r="BI4" s="111">
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="114"/>
+      <c r="BH4" s="115"/>
+      <c r="BI4" s="113">
         <f>BI5</f>
         <v>44872</v>
       </c>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="112"/>
-      <c r="BO4" s="113"/>
-      <c r="BP4" s="111">
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="114"/>
+      <c r="BO4" s="115"/>
+      <c r="BP4" s="113">
         <f>BP5</f>
         <v>44879</v>
       </c>
-      <c r="BQ4" s="112"/>
-      <c r="BR4" s="112"/>
-      <c r="BS4" s="112"/>
-      <c r="BT4" s="112"/>
-      <c r="BU4" s="112"/>
-      <c r="BV4" s="113"/>
-      <c r="BW4" s="111">
+      <c r="BQ4" s="114"/>
+      <c r="BR4" s="114"/>
+      <c r="BS4" s="114"/>
+      <c r="BT4" s="114"/>
+      <c r="BU4" s="114"/>
+      <c r="BV4" s="115"/>
+      <c r="BW4" s="113">
         <f>BW5</f>
         <v>44886</v>
       </c>
-      <c r="BX4" s="112"/>
-      <c r="BY4" s="112"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="113"/>
+      <c r="BX4" s="114"/>
+      <c r="BY4" s="114"/>
+      <c r="BZ4" s="114"/>
+      <c r="CA4" s="114"/>
+      <c r="CB4" s="114"/>
+      <c r="CC4" s="115"/>
     </row>
     <row r="5" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="D29" s="67"/>
       <c r="E29" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="93">
         <f>DATE(2022,11,14)</f>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="D30" s="67"/>
       <c r="E30" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="93">
         <f>F29</f>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="D35" s="81"/>
       <c r="E35" s="82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="96">
         <f>F30</f>
@@ -6143,7 +6143,10 @@
         <f>DATE(2022,10,21)</f>
         <v>44855</v>
       </c>
-      <c r="I35" s="96"/>
+      <c r="I35" s="96">
+        <f>H35</f>
+        <v>44855</v>
+      </c>
       <c r="J35" s="17"/>
       <c r="K35" s="17">
         <f t="shared" si="17"/>
@@ -6712,11 +6715,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="AN4:AT4"/>
-    <mergeCell ref="AU4:BA4"/>
-    <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BP4:BV4"/>
     <mergeCell ref="BW4:CC4"/>
     <mergeCell ref="BI4:BO4"/>
@@ -6725,6 +6723,11 @@
     <mergeCell ref="S4:Y4"/>
     <mergeCell ref="Z4:AF4"/>
     <mergeCell ref="AG4:AM4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="AN4:AT4"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="BB4:BH4"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E40">
     <cfRule type="dataBar" priority="71">

</xml_diff>

<commit_message>
Documentation changes & embedded fixes attempts
</commit_message>
<xml_diff>
--- a/References/Tidsplan.xlsx
+++ b/References/Tidsplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5BE65F-8A8A-4DCC-BC9A-5E393326CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68178F56-78CE-4CCE-9AEE-1C8339CADD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,9 +344,6 @@
     <t>T13</t>
   </si>
   <si>
-    <t>Smart vægt</t>
-  </si>
-  <si>
     <t>Daniel Simonsen</t>
   </si>
   <si>
@@ -458,6 +455,9 @@
       </rPr>
       <t xml:space="preserve"> - RedisCache til API cache - evt. Container</t>
     </r>
+  </si>
+  <si>
+    <t>SmartWeight</t>
   </si>
 </sst>
 </file>
@@ -1240,6 +1240,12 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1251,12 +1257,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2267,13 +2267,13 @@
         <v>68</v>
       </c>
       <c r="F6" s="101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>72</v>
@@ -2282,7 +2282,7 @@
         <v>68</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>74</v>
@@ -2312,13 +2312,13 @@
         <v>68</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>74</v>
@@ -2327,7 +2327,7 @@
         <v>68</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -2372,7 +2372,7 @@
         <v>68</v>
       </c>
       <c r="F13" s="101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -2465,7 +2465,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>74</v>
@@ -2474,12 +2474,12 @@
         <v>70</v>
       </c>
       <c r="F20" s="101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>71</v>
@@ -2488,7 +2488,7 @@
         <v>70</v>
       </c>
       <c r="F21" s="101" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -2576,9 +2576,9 @@
   </sheetPr>
   <dimension ref="A1:CC43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CD3" sqref="CD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L2" s="104" t="s">
         <v>19</v>
@@ -2632,129 +2632,129 @@
       </c>
       <c r="B3" s="58"/>
       <c r="C3" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="116"/>
-      <c r="F3" s="114">
+      <c r="E3" s="112"/>
+      <c r="F3" s="116">
         <f>DATE(2022,9,19)</f>
         <v>44823</v>
       </c>
-      <c r="G3" s="114"/>
+      <c r="G3" s="116"/>
     </row>
     <row r="4" spans="1:81" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="116"/>
+      <c r="E4" s="112"/>
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="111">
+      <c r="L4" s="113">
         <f>L5</f>
         <v>44823</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="111">
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="113">
         <f>S5</f>
         <v>44830</v>
       </c>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="113"/>
-      <c r="Z4" s="111">
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="114"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="113">
         <f>Z5</f>
         <v>44837</v>
       </c>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="113"/>
-      <c r="AG4" s="111">
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="114"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="113">
         <f>AG5</f>
         <v>44844</v>
       </c>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="112"/>
-      <c r="AM4" s="113"/>
-      <c r="AN4" s="111">
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="114"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="113">
         <f>AN5</f>
         <v>44851</v>
       </c>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="112"/>
-      <c r="AT4" s="113"/>
-      <c r="AU4" s="111">
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="114"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="113">
         <f>AU5</f>
         <v>44858</v>
       </c>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="112"/>
-      <c r="BA4" s="113"/>
-      <c r="BB4" s="111">
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="114"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="113">
         <f>BB5</f>
         <v>44865</v>
       </c>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="112"/>
-      <c r="BH4" s="113"/>
-      <c r="BI4" s="111">
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="114"/>
+      <c r="BH4" s="115"/>
+      <c r="BI4" s="113">
         <f>BI5</f>
         <v>44872</v>
       </c>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="112"/>
-      <c r="BO4" s="113"/>
-      <c r="BP4" s="111">
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="114"/>
+      <c r="BO4" s="115"/>
+      <c r="BP4" s="113">
         <f>BP5</f>
         <v>44879</v>
       </c>
-      <c r="BQ4" s="112"/>
-      <c r="BR4" s="112"/>
-      <c r="BS4" s="112"/>
-      <c r="BT4" s="112"/>
-      <c r="BU4" s="112"/>
-      <c r="BV4" s="113"/>
-      <c r="BW4" s="111">
+      <c r="BQ4" s="114"/>
+      <c r="BR4" s="114"/>
+      <c r="BS4" s="114"/>
+      <c r="BT4" s="114"/>
+      <c r="BU4" s="114"/>
+      <c r="BV4" s="115"/>
+      <c r="BW4" s="113">
         <f>BW5</f>
         <v>44886</v>
       </c>
-      <c r="BX4" s="112"/>
-      <c r="BY4" s="112"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="113"/>
+      <c r="BX4" s="114"/>
+      <c r="BY4" s="114"/>
+      <c r="BZ4" s="114"/>
+      <c r="CA4" s="114"/>
+      <c r="CB4" s="114"/>
+      <c r="CC4" s="115"/>
     </row>
     <row r="5" spans="1:81" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
@@ -3055,7 +3055,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>11</v>
@@ -3071,10 +3071,10 @@
         <v>8</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
@@ -3740,7 +3740,7 @@
       <c r="CB10" s="99"/>
       <c r="CC10" s="99"/>
     </row>
-    <row r="11" spans="1:81" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:81" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52"/>
       <c r="B11" s="69"/>
       <c r="C11" s="69" t="s">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="D12" s="61"/>
       <c r="E12" s="22">
-        <v>0.15</v>
+        <v>0.9</v>
       </c>
       <c r="F12" s="84">
         <f>DATE(2022,9,30)</f>
@@ -3936,11 +3936,11 @@
       <c r="A13" s="52"/>
       <c r="B13" s="69"/>
       <c r="C13" s="69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="61"/>
       <c r="E13" s="22">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F13" s="84">
         <f>F25</f>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="28">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="F23" s="90">
         <f>DATE(2022,10,12)</f>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="D24" s="65"/>
       <c r="E24" s="28">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F24" s="90">
         <f>DATE(2022,10,12)</f>
@@ -5058,7 +5058,10 @@
         <f>H23</f>
         <v>44855</v>
       </c>
-      <c r="I24" s="90"/>
+      <c r="I24" s="90">
+        <f>DATE(2022,11,2)</f>
+        <v>44867</v>
+      </c>
       <c r="J24" s="17"/>
       <c r="K24" s="17">
         <f t="shared" si="17"/>
@@ -6718,11 +6721,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="AN4:AT4"/>
-    <mergeCell ref="AU4:BA4"/>
-    <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BP4:BV4"/>
     <mergeCell ref="BW4:CC4"/>
     <mergeCell ref="BI4:BO4"/>
@@ -6731,6 +6729,11 @@
     <mergeCell ref="S4:Y4"/>
     <mergeCell ref="Z4:AF4"/>
     <mergeCell ref="AG4:AM4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="AN4:AT4"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="BB4:BH4"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E40">
     <cfRule type="dataBar" priority="71">
@@ -6939,7 +6942,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="40" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -6987,19 +6990,19 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="109" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="109" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="C1" s="109" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="109" t="s">
-        <v>107</v>
       </c>
       <c r="D1" s="110"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="107">
         <v>3</v>
@@ -7013,7 +7016,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="107">
         <v>5</v>
@@ -7027,7 +7030,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="107">
         <v>2</v>
@@ -7041,7 +7044,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="107">
         <v>2</v>
@@ -7055,7 +7058,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="107">
         <v>2</v>
@@ -7069,7 +7072,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="106" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="107">
         <v>1</v>
@@ -7083,7 +7086,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="107">
         <v>4</v>
@@ -7097,7 +7100,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="107">
         <v>4</v>
@@ -7111,7 +7114,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="107">
         <v>1</v>
@@ -7125,7 +7128,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="106" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="107">
         <v>1</v>

</xml_diff>